<commit_message>
latest lit review updates
</commit_message>
<xml_diff>
--- a/CLEO_2023/lit_review.xlsx
+++ b/CLEO_2023/lit_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterchang/Github/Microscope_Data_Analysis/CLEO_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277FE9B1-9C5D-D24F-BB75-520A2E6A9820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF2A8AF-1A93-8341-83F3-E444A84A31CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="880" windowWidth="23340" windowHeight="16480" xr2:uid="{AC1D25CF-D65A-3447-B781-019695790FE4}"/>
+    <workbookView xWindow="3040" yWindow="660" windowWidth="23340" windowHeight="16480" xr2:uid="{AC1D25CF-D65A-3447-B781-019695790FE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Publication</t>
   </si>
@@ -54,13 +54,46 @@
   </si>
   <si>
     <t>single wavelength</t>
+  </si>
+  <si>
+    <t>Spectral Resolution</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Single Spectra Acquisition time</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">M. Tamamitsu et al., Vibrational Spectroscopy </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>91</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, 163 (2017)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,6 +111,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -104,12 +152,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,39 +474,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0290F9B0-6CA7-A343-B369-B8265A002920}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>